<commit_message>
feat: upload to cloudinary
</commit_message>
<xml_diff>
--- a/apps/server/templates/siswa-template.xlsx
+++ b/apps/server/templates/siswa-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farriq\Documents\Projects\stay\apps\server\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAF6453-F7C6-478D-B07B-0CA225CA779F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D40C63B-8582-4E03-A4F4-649582685847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD4919B6-CA53-4B5F-AB66-0848646E9413}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>notelp</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>rombel</t>
+  </si>
+  <si>
+    <t>image_url</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2533E3BC-4B6D-47F3-8C5C-ACFC68E4C00C}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:H8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,9 +455,10 @@
     <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,9 +473,13 @@
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>